<commit_message>
add minSCe single cell templates transcriptomics tag
</commit_message>
<xml_diff>
--- a/templates/dataplant/minSCe/minSCe_-_Data_analysis.xlsx
+++ b/templates/dataplant/minSCe/minSCe_-_Data_analysis.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t xml:space="preserve">TEMPLATE</t>
   </si>
@@ -92,6 +92,9 @@
     <t xml:space="preserve">minSCe</t>
   </si>
   <si>
+    <t xml:space="preserve">Transcriptomics</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tags Term Accession Number</t>
   </si>
   <si>
@@ -104,6 +107,9 @@
     <t xml:space="preserve">https://bioregistry.io/NCIT:C184799</t>
   </si>
   <si>
+    <t xml:space="preserve">https://bioregistry.io/NCIT:C153189</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tags Term Source REF</t>
   </si>
   <si>
@@ -123,6 +129,9 @@
   </si>
   <si>
     <t xml:space="preserve">"Any data from investigations or experiments performed on samples derived from single cells." []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"A study of the complete set of RNA transcripts that are produced by the genome, under specific circumstances or in a specific cell." []</t>
   </si>
   <si>
     <t xml:space="preserve">Comment[isObsolete]</t>
@@ -416,258 +425,273 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>35</v>
+      <c r="F16" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>36</v>
+      <c r="A18" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>38</v>
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>40</v>
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>41</v>
+      <c r="A21" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>43</v>
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>45</v>
+      <c r="A23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>46</v>
+      <c r="A24" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>48</v>
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>50</v>
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>52</v>
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>54</v>
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>56</v>
+      <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>58</v>
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -689,91 +713,91 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F13:F17 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>83</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>